<commit_message>
Modal + New Wallpaper
</commit_message>
<xml_diff>
--- a/downpaper/wallpaper/wallpaper.xlsx
+++ b/downpaper/wallpaper/wallpaper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEREN\Project\DownPaper\DownPaper\storage\app\public\wallpaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE2558F-ADCB-4A67-9072-546B2A7E55A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F648D332-E4B7-42CD-BB90-EEEED3B1ECC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10416" yWindow="324" windowWidth="13164" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1092" yWindow="1128" windowWidth="13164" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Birthday</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Boat</t>
   </si>
   <si>
-    <t>Just a birthday at the squad's home.</t>
-  </si>
-  <si>
     <t>The squad is on the boat and please focus on Ethen.</t>
   </si>
   <si>
@@ -135,31 +132,70 @@
     <t>Celebrating a lot of racers are moving in this competitive village.</t>
   </si>
   <si>
-    <t>Did you know that this day honors Saint Valentine who was martyred in 269?</t>
-  </si>
-  <si>
     <t>Who lives in a pineapple under the sea?</t>
   </si>
   <si>
     <t>RUN RUN RUN RUN RUN RUN RUN RUN RUN RUN.</t>
   </si>
   <si>
-    <t>The most badass wallpaper ever. I bought my Saber Hellfire because of this and also, ever since this, I learn fullstack webdev.</t>
-  </si>
-  <si>
-    <t>If Dao is the champion, I am &lt;a href="https://github.com/taylorotwell"&gt;Taylor Otwell&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Just a nice day on December 31st 23:59PM.</t>
-  </si>
-  <si>
     <t>Another badass wallpaper from Season 4 that I love and as badass as the previous one.</t>
   </si>
   <si>
-    <t>Next time, use Uber, you blue little boy.</t>
-  </si>
-  <si>
     <t>The fight has already began. Please watch on how both of them will annihilate other.</t>
+  </si>
+  <si>
+    <t>16.jpg</t>
+  </si>
+  <si>
+    <t>17.jpg</t>
+  </si>
+  <si>
+    <t>18.jpg</t>
+  </si>
+  <si>
+    <t>19.jpg</t>
+  </si>
+  <si>
+    <t>3… 2… 1… GO!</t>
+  </si>
+  <si>
+    <t>Autumn Exploration</t>
+  </si>
+  <si>
+    <t>Winter for Winners</t>
+  </si>
+  <si>
+    <t>CNY Cooking Time</t>
+  </si>
+  <si>
+    <t>Bazzi is sleeping, the couple is picking a bunch of apples, Uni transports them, and Ethen? Finding something interesting?</t>
+  </si>
+  <si>
+    <t>Going outside to do a fun activities. Racing is fun, but not always be a primary source of fun. Take snowman assembling or skating for example :)</t>
+  </si>
+  <si>
+    <t>Yummy… what meat is that? Cuz I am quite allergic to seafood :(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The most badass wallpaper ever. I bought my Saber Hellfire because of this, setting this to be my PC wallpaper, and also ever since this was discovered, I learn fullstack webdev (useless coincidental fact for you). </t>
+  </si>
+  <si>
+    <t>Just a birthday at the squad's home. Happy Birthday, Dao.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just a nice day on December 31st 23:59PM. </t>
+  </si>
+  <si>
+    <t>If Dao is the champion versus the player, I am &lt;a href=\"https://github.com/taylorotwell\"&gt;Taylor Otwell&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Next time, use Uber, you blue little boy. You do own your own phone, am I right?</t>
+  </si>
+  <si>
+    <t>Did you know that this day honors Saint Valentine who was martyred in 269 AD?</t>
+  </si>
+  <si>
+    <t>Lodu still do the heck anywhere and its time for The Squad to end this once and for all.</t>
   </si>
 </sst>
 </file>
@@ -480,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,8 +538,8 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -516,8 +552,8 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -525,41 +561,41 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -567,13 +603,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>42</v>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,13 +617,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -595,13 +631,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -609,13 +645,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -623,13 +659,13 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
-        <v>33</v>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -637,13 +673,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>34</v>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -651,13 +687,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
-        <v>35</v>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,13 +701,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
-        <v>36</v>
+      <c r="D13" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -679,13 +715,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
-        <v>37</v>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -693,13 +729,69 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
-        <v>38</v>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>